<commit_message>
Fix issue with converting type of questions
</commit_message>
<xml_diff>
--- a/fieldManagerClient/WebContent/blankform.xlsx
+++ b/fieldManagerClient/WebContent/blankform.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="14200" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="14200"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -475,11 +475,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -605,7 +605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated xlsform template to include display_name for choices
</commit_message>
<xml_diff>
--- a/fieldManagerClient/WebContent/blankform.xlsx
+++ b/fieldManagerClient/WebContent/blankform.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="14200"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14140"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>type</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>display_name</t>
   </si>
 </sst>
 </file>
@@ -475,7 +478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -566,21 +569,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1:F1048576"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="3" width="20" customWidth="1"/>
+    <col min="1" max="4" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -588,6 +591,9 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Give users with admin rights access to the console
</commit_message>
<xml_diff>
--- a/fieldManagerClient/WebContent/blankform.xlsx
+++ b/fieldManagerClient/WebContent/blankform.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14140"/>
+    <workbookView xWindow="480" yWindow="920" windowWidth="25120" windowHeight="13220"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="2" r:id="rId2"/>
     <sheet name="settings" sheetId="3" r:id="rId3"/>
+    <sheet name="styles" sheetId="4" r:id="rId4"/>
+    <sheet name="conditions" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>type</t>
   </si>
@@ -35,6 +37,12 @@
     <t>hint::language</t>
   </si>
   <si>
+    <t>guidance_hint::language</t>
+  </si>
+  <si>
+    <t>display_name</t>
+  </si>
+  <si>
     <t>choice_filter</t>
   </si>
   <si>
@@ -68,6 +76,9 @@
     <t>body::accuracyThreshold</t>
   </si>
   <si>
+    <t>body::intent</t>
+  </si>
+  <si>
     <t>required</t>
   </si>
   <si>
@@ -77,31 +88,70 @@
     <t>calculation</t>
   </si>
   <si>
-    <t>image::language</t>
-  </si>
-  <si>
-    <t>video::language</t>
-  </si>
-  <si>
-    <t>audio::language</t>
+    <t>style list</t>
+  </si>
+  <si>
+    <t>media::image::language</t>
+  </si>
+  <si>
+    <t>media::video::language</t>
+  </si>
+  <si>
+    <t>media::audio::language</t>
+  </si>
+  <si>
+    <t>list_name</t>
+  </si>
+  <si>
+    <t>default_language</t>
+  </si>
+  <si>
+    <t>instance_name</t>
+  </si>
+  <si>
+    <t>style</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>key_policy</t>
+  </si>
+  <si>
+    <t>allow_import</t>
+  </si>
+  <si>
+    <t>hide_on_device</t>
+  </si>
+  <si>
+    <t>timing_data</t>
+  </si>
+  <si>
+    <t>audit_location_data</t>
+  </si>
+  <si>
+    <t>track_changes</t>
+  </si>
+  <si>
+    <t>pulldata_repeat</t>
   </si>
   <si>
     <t>list name</t>
   </si>
   <si>
-    <t>default_language</t>
-  </si>
-  <si>
-    <t>instance_name</t>
-  </si>
-  <si>
-    <t>style</t>
+    <t>value</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>question name</t>
+  </si>
+  <si>
+    <t>rule</t>
   </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t>display_name</t>
   </si>
 </sst>
 </file>
@@ -476,23 +526,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="40" customWidth="1"/>
-    <col min="4" max="21" width="20" customWidth="1"/>
+    <col min="4" max="25" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -555,6 +605,18 @@
       </c>
       <c r="U1" s="1" t="s">
         <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -569,32 +631,41 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="4" width="20" customWidth="1"/>
+    <col min="1" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -609,11 +680,75 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="G1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="11" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -622,18 +757,45 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="B2" t="s">
-        <v>25</v>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="3" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add server_calculation to templater
</commit_message>
<xml_diff>
--- a/fieldManagerClient/WebContent/blankform.xlsx
+++ b/fieldManagerClient/WebContent/blankform.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
   <si>
     <t>type</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>server_calculation</t>
   </si>
 </sst>
 </file>
@@ -526,23 +529,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="40" customWidth="1"/>
-    <col min="4" max="25" width="20" customWidth="1"/>
+    <col min="4" max="26" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -607,15 +610,18 @@
         <v>20</v>
       </c>
       <c r="V1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove display_name column from choices sheet
</commit_message>
<xml_diff>
--- a/fieldManagerClient/WebContent/blankform.xlsx
+++ b/fieldManagerClient/WebContent/blankform.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t>type</t>
   </si>
@@ -532,7 +532,7 @@
   <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="V2" sqref="V2"/>
@@ -637,21 +637,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="7" width="20" customWidth="1"/>
+    <col min="1" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -659,18 +659,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Simplified xls template with some language settings removed
</commit_message>
<xml_diff>
--- a/fieldManagerClient/WebContent/blankform.xlsx
+++ b/fieldManagerClient/WebContent/blankform.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="920" windowWidth="25120" windowHeight="13220"/>
+    <workbookView xWindow="480" yWindow="920" windowWidth="25120" windowHeight="13220" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -37,9 +37,6 @@
     <t>hint::language</t>
   </si>
   <si>
-    <t>guidance_hint::language</t>
-  </si>
-  <si>
     <t>display_name</t>
   </si>
   <si>
@@ -91,15 +88,6 @@
     <t>style list</t>
   </si>
   <si>
-    <t>media::image::language</t>
-  </si>
-  <si>
-    <t>media::video::language</t>
-  </si>
-  <si>
-    <t>media::audio::language</t>
-  </si>
-  <si>
     <t>list_name</t>
   </si>
   <si>
@@ -155,6 +143,18 @@
   </si>
   <si>
     <t>server_calculation</t>
+  </si>
+  <si>
+    <t>guidance_hint</t>
+  </si>
+  <si>
+    <t>media::image</t>
+  </si>
+  <si>
+    <t>media::video</t>
+  </si>
+  <si>
+    <t>media::audio</t>
   </si>
 </sst>
 </file>
@@ -531,11 +531,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="V2" sqref="V2"/>
+      <selection pane="bottomRight" activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -559,70 +559,70 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -639,11 +639,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -653,7 +653,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -662,13 +662,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -696,45 +696,45 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="B2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="K2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -760,13 +760,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -792,13 +792,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update blankform to open on the survey sheet
</commit_message>
<xml_diff>
--- a/fieldManagerClient/WebContent/blankform.xlsx
+++ b/fieldManagerClient/WebContent/blankform.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="920" windowWidth="25120" windowHeight="13220" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="920" windowWidth="25120" windowHeight="13220"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -531,11 +531,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="X1" sqref="X1"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -639,7 +639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>

</xml_diff>

<commit_message>
Removed language defaults from template
</commit_message>
<xml_diff>
--- a/fieldManagerClient/WebContent/blankform.xlsx
+++ b/fieldManagerClient/WebContent/blankform.xlsx
@@ -31,12 +31,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>label::language</t>
-  </si>
-  <si>
-    <t>hint::language</t>
-  </si>
-  <si>
     <t>display_name</t>
   </si>
   <si>
@@ -155,6 +149,12 @@
   </si>
   <si>
     <t>media::audio</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>hint</t>
   </si>
 </sst>
 </file>
@@ -532,10 +532,10 @@
   <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -553,76 +553,76 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -643,7 +643,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -653,22 +653,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -696,45 +696,45 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="B2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -760,13 +760,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -792,13 +792,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update blankform with selectable types
</commit_message>
<xml_diff>
--- a/fieldManagerClient/WebContent/blankform.xlsx
+++ b/fieldManagerClient/WebContent/blankform.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10917"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neilpenman/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93760ADC-697B-B64E-B1FB-AA2355F5FE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="920" windowWidth="25120" windowHeight="13220"/>
+    <workbookView xWindow="480" yWindow="920" windowWidth="30680" windowHeight="13220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -12,9 +18,21 @@
     <sheet name="settings" sheetId="3" r:id="rId3"/>
     <sheet name="styles" sheetId="4" r:id="rId4"/>
     <sheet name="conditions" sheetId="5" r:id="rId5"/>
+    <sheet name="Types" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -23,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="116">
   <si>
     <t>type</t>
   </si>
@@ -155,13 +173,229 @@
   </si>
   <si>
     <t>hint</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>calculate</t>
+  </si>
+  <si>
+    <t>select_one list_name</t>
+  </si>
+  <si>
+    <t>select_multiple list_name</t>
+  </si>
+  <si>
+    <t>begin_repeat</t>
+  </si>
+  <si>
+    <t>end_repeat</t>
+  </si>
+  <si>
+    <t>begin_group</t>
+  </si>
+  <si>
+    <t>end_group</t>
+  </si>
+  <si>
+    <t>geopoint</t>
+  </si>
+  <si>
+    <t>geotrace</t>
+  </si>
+  <si>
+    <t>geoshape</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>barcode</t>
+  </si>
+  <si>
+    <t>audio</t>
+  </si>
+  <si>
+    <t>background-audio</t>
+  </si>
+  <si>
+    <t>video</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>rank</t>
+  </si>
+  <si>
+    <t>acknowledge</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>A text response</t>
+  </si>
+  <si>
+    <t>Show information to the user</t>
+  </si>
+  <si>
+    <t>An integer response. Do not use for phone numbers. Instead use text with an appearance of numbers</t>
+  </si>
+  <si>
+    <t>A decimal response</t>
+  </si>
+  <si>
+    <t>bearing</t>
+  </si>
+  <si>
+    <t>Captures the compass reading</t>
+  </si>
+  <si>
+    <t>Scan a barcode</t>
+  </si>
+  <si>
+    <t>nfc</t>
+  </si>
+  <si>
+    <t>Scan an NFC chiip</t>
+  </si>
+  <si>
+    <t>Date without time</t>
+  </si>
+  <si>
+    <t>Just the time</t>
+  </si>
+  <si>
+    <t>Date and time</t>
+  </si>
+  <si>
+    <t>Calculate a value from answers</t>
+  </si>
+  <si>
+    <t>Select a single value from a list</t>
+  </si>
+  <si>
+    <t>Select multiple values from a list</t>
+  </si>
+  <si>
+    <t>Add an image using the camera or from stored photos.</t>
+  </si>
+  <si>
+    <t>The start of a subform containing questions that are repeated</t>
+  </si>
+  <si>
+    <t>The end of a sub form</t>
+  </si>
+  <si>
+    <t>The start of a group of questions</t>
+  </si>
+  <si>
+    <t>The end of a group of questions</t>
+  </si>
+  <si>
+    <t>chart</t>
+  </si>
+  <si>
+    <t>Show data as a chart to the user</t>
+  </si>
+  <si>
+    <t>Record the coordinates of a point</t>
+  </si>
+  <si>
+    <t>Record the coordinates of a line</t>
+  </si>
+  <si>
+    <t>Record the coordinates of an area</t>
+  </si>
+  <si>
+    <t>Select a value within a ranve</t>
+  </si>
+  <si>
+    <t>Revord audio</t>
+  </si>
+  <si>
+    <t>Automatically record audio while the survey is being completed</t>
+  </si>
+  <si>
+    <t>Record a video</t>
+  </si>
+  <si>
+    <t>Attach a file</t>
+  </si>
+  <si>
+    <t>begin matrix</t>
+  </si>
+  <si>
+    <t>end matrix</t>
+  </si>
+  <si>
+    <t>The start of questions that are shown as a matrix</t>
+  </si>
+  <si>
+    <t>The end of questions that are shown as a matrix</t>
+  </si>
+  <si>
+    <t>FieldTask</t>
+  </si>
+  <si>
+    <t>WebForms</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Rank a list of choices</t>
+  </si>
+  <si>
+    <t>Require the user to acknowledge a statement before proceeding</t>
+  </si>
+  <si>
+    <t>server_calculate</t>
+  </si>
+  <si>
+    <t>Calculations that are done on the server when the data is viewed</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>&lt;h1&gt;x&lt;/h1&gt;&lt;script&gt;alert("hi");&lt;/script&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -173,19 +407,52 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -195,15 +462,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -528,24 +815,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <tabColor theme="6" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="40" customWidth="1"/>
     <col min="4" max="26" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -623,11 +913,44 @@
       </c>
       <c r="Z1" s="1" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" t="s">
+        <v>115</v>
+      </c>
+      <c r="I3" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{E16096F3-06AE-F541-9177-A9F82C0D0CE4}">
+          <x14:formula1>
+            <xm:f>Types!$A$3:$A$34</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2:A200</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
@@ -636,22 +959,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <tabColor theme="6" tint="0.39997558519241921"/>
+  </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -682,19 +1008,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
+    <tabColor theme="6" tint="0.39997558519241921"/>
+  </sheetPr>
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView topLeftCell="G1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="11" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -729,7 +1058,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>36</v>
       </c>
@@ -748,17 +1077,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.39997558519241921"/>
+  </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -780,17 +1114,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.39997558519241921"/>
+  </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -809,4 +1146,488 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6204A07-98BF-3241-9CD0-6A700EA9E4DB}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A2:D34"/>
+  <sheetViews>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="I51" sqref="I51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Remove sample question from blankform
</commit_message>
<xml_diff>
--- a/fieldManagerClient/WebContent/blankform.xlsx
+++ b/fieldManagerClient/WebContent/blankform.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neilpenman/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neilpenman/git/prop-smapserver/fieldManagerClient/WebContent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93760ADC-697B-B64E-B1FB-AA2355F5FE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1299FB0-2B5E-C248-918F-9C53F73FC192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="920" windowWidth="30680" windowHeight="13220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="920" windowWidth="30680" windowHeight="13220" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="114">
   <si>
     <t>type</t>
   </si>
@@ -383,12 +383,6 @@
   </si>
   <si>
     <t>Calculations that are done on the server when the data is viewed</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>&lt;h1&gt;x&lt;/h1&gt;&lt;script&gt;alert("hi");&lt;/script&gt;</t>
   </si>
 </sst>
 </file>
@@ -468,13 +462,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -819,13 +813,13 @@
   <sheetPr>
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -915,29 +909,6 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E3" t="s">
-        <v>115</v>
-      </c>
-      <c r="F3" t="s">
-        <v>115</v>
-      </c>
-      <c r="I3" t="s">
-        <v>115</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -947,7 +918,7 @@
           <x14:formula1>
             <xm:f>Types!$A$3:$A$34</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A200</xm:sqref>
+          <xm:sqref>A2:A199</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1155,7 +1126,7 @@
   </sheetPr>
   <dimension ref="A2:D34"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Set initial worksheeet to survey
</commit_message>
<xml_diff>
--- a/fieldManagerClient/WebContent/blankform.xlsx
+++ b/fieldManagerClient/WebContent/blankform.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neilpenman/git/prop-smapserver/fieldManagerClient/WebContent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1299FB0-2B5E-C248-918F-9C53F73FC192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555B6DA2-2CB2-E047-9B8E-864FB036E234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="920" windowWidth="30680" windowHeight="13220" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="920" windowWidth="30680" windowHeight="13220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -815,11 +815,11 @@
   </sheetPr>
   <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:XFD3"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1126,7 +1126,7 @@
   </sheetPr>
   <dimension ref="A2:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>

</xml_diff>